<commit_message>
BWP Test Cases Added
</commit_message>
<xml_diff>
--- a/KatalonData/BWPBootstrapData/EmulatorNormalizedData.xlsx
+++ b/KatalonData/BWPBootstrapData/EmulatorNormalizedData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\VPS-Katalon-feature-VRelay\KatalonData\BWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41AE090-715A-435F-B754-91749376B822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E3D56F-DEE9-4B6C-BC99-A972F32969A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="46">
   <si>
     <t>MV</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>SingleCFPercentage</t>
+  </si>
+  <si>
+    <t>MissingReqFields</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,6 +1314,23 @@
         <v>33</v>
       </c>
     </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>950</v>
+      </c>
+      <c r="D18">
+        <v>1.5</v>
+      </c>
+      <c r="O18" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>